<commit_message>
2024 09 10 밀린 커밋
</commit_message>
<xml_diff>
--- a/인프런.xlsx
+++ b/인프런.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mwzz6\Desktop\GITHUB\Inflearn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65FAA924-79C8-46AF-BEC4-E1283CDD81BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA5FF19-02FF-480A-A647-BC73F5FCE103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3100" yWindow="790" windowWidth="19200" windowHeight="11260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="43">
   <si>
     <t>섹션 0</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1168,10 +1168,16 @@
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -1181,11 +1187,11 @@
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
+      <c r="O16" s="4"/>
       <c r="P16" s="4"/>
     </row>
     <row r="17" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="8" t="s">
@@ -1200,10 +1206,18 @@
       <c r="E17" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
+      <c r="F17" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>

</xml_diff>